<commit_message>
NN small and big finished
</commit_message>
<xml_diff>
--- a/NN_output/GM12878/Small_classification_report.xlsx
+++ b/NN_output/GM12878/Small_classification_report.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7923280423280423</v>
+        <v>0.7463439233484619</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5084889643463497</v>
+        <v>0.6281833616298812</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6194415718717684</v>
+        <v>0.6821848352154875</v>
       </c>
       <c r="E2" t="n">
         <v>2356</v>
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4272997032640949</v>
+        <v>0.4352030947775629</v>
       </c>
       <c r="C3" t="n">
-        <v>0.733446519524618</v>
+        <v>0.5730050933786078</v>
       </c>
       <c r="D3" t="n">
-        <v>0.54</v>
+        <v>0.4946866984243313</v>
       </c>
       <c r="E3" t="n">
         <v>1178</v>
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5834748160724391</v>
+        <v>0.6097906055461234</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5834748160724391</v>
+        <v>0.6097906055461234</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5834748160724391</v>
+        <v>0.6097906055461234</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5834748160724391</v>
+        <v>0.6097906055461234</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6098138727960687</v>
+        <v>0.5907735090630124</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6209677419354839</v>
+        <v>0.6005942275042445</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5797207859358842</v>
+        <v>0.5884357668199094</v>
       </c>
       <c r="E5" t="n">
         <v>3534</v>
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6706519293067266</v>
+        <v>0.6426303138248289</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5834748160724391</v>
+        <v>0.6097906055461234</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5929610479145123</v>
+        <v>0.6196854562851021</v>
       </c>
       <c r="E6" t="n">
         <v>3534</v>

</xml_diff>